<commit_message>
added new column 'result' in test_data.xlsx
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Sr.No</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Player3</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -414,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,8 +441,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -443,8 +455,11 @@
       <c r="C2" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -454,8 +469,11 @@
       <c r="C3" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -465,8 +483,11 @@
       <c r="C4" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -476,8 +497,11 @@
       <c r="C5" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -487,8 +511,11 @@
       <c r="C6" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -498,8 +525,11 @@
       <c r="C7" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -509,8 +539,11 @@
       <c r="C8" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -520,8 +553,11 @@
       <c r="C9" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -531,8 +567,11 @@
       <c r="C10" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -542,8 +581,11 @@
       <c r="C11" s="2">
         <v>110</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -553,8 +595,11 @@
       <c r="C12" s="2">
         <v>120</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -563,6 +608,9 @@
       </c>
       <c r="C13" s="2">
         <v>130</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the color of result column
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -96,7 +96,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +106,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,12 +143,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +433,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +462,7 @@
       <c r="C2" s="2">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -469,7 +476,7 @@
       <c r="C3" s="2">
         <v>30</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -483,7 +490,7 @@
       <c r="C4" s="2">
         <v>40</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -497,7 +504,7 @@
       <c r="C5" s="2">
         <v>50</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -511,7 +518,7 @@
       <c r="C6" s="2">
         <v>60</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -525,7 +532,7 @@
       <c r="C7" s="2">
         <v>70</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -539,7 +546,7 @@
       <c r="C8" s="2">
         <v>80</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -553,7 +560,7 @@
       <c r="C9" s="2">
         <v>90</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -567,7 +574,7 @@
       <c r="C10" s="2">
         <v>100</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -581,7 +588,7 @@
       <c r="C11" s="2">
         <v>110</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -595,7 +602,7 @@
       <c r="C12" s="2">
         <v>120</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -609,7 +616,7 @@
       <c r="C13" s="2">
         <v>130</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed color of column 2 in sheet 1
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,6 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +477,7 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2">
@@ -484,7 +491,7 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2">
@@ -498,7 +505,7 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2">
@@ -512,7 +519,7 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2">
@@ -526,7 +533,7 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2">
@@ -540,7 +547,7 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2">
@@ -554,7 +561,7 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="2">
@@ -568,7 +575,7 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2">
@@ -582,7 +589,7 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="2">
@@ -596,7 +603,7 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2">
@@ -610,7 +617,7 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2">
@@ -644,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>